<commit_message>
Enviando e-mail e finalizando o Projeto
</commit_message>
<xml_diff>
--- a/Ofertas.xlsx
+++ b/Ofertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>produto</t>
   </si>
@@ -25,7 +25,7 @@
     <t>link</t>
   </si>
   <si>
-    <t>apple iphone 12 64gb preto 5g tela 6,1" câm. traseira 12+12mp frontal 12mp</t>
+    <t>smartphone apple iphone 12, 64gb, branco, 5g, 6.1" super retina xdr oled, câmera dupla 12mp, selfie 12mp, ios 15</t>
   </si>
   <si>
     <t>iphone 12 64gb roxo tela 6,1 4g câmera traseira 12mp vitrine</t>
@@ -34,7 +34,16 @@
     <t>vitrine iphone 12 preto 64gb</t>
   </si>
   <si>
-    <t>smartphone apple iphone 12, 64gb, branco, 5g, 6.1" super retina xdr oled, câmera dupla 12mp, selfie 12mp, ios 15</t>
+    <t>iphone 12 64gb preto de vitrine tela 6,1 4g câmera traseira 12mp 12mp vitrine</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb branco de vitrine tela 6,1&amp;quot; 4g câmera traseira 12mp+12mp - vitrine</t>
+  </si>
+  <si>
+    <t>vitrine iphone 12 verde 64gb</t>
+  </si>
+  <si>
+    <t>celular apple iphone 12 black 64gb vitrine/seminovo com carrregador e cabo</t>
   </si>
   <si>
     <t>smartphone apple iphone 12 64gb câmera dupla</t>
@@ -43,16 +52,25 @@
     <t>placa de video nvidia geforce rtx 3060 ti 8 gb gddr6 192 bits asus dual-rtx3060ti-o8g-v2</t>
   </si>
   <si>
-    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwiayt_c7b2AAxXIMdQBHZwOArIYABABGgJvYQ&amp;gclid=EAIaIQobChMImsrf3O29gAMVyDHUAR2cDgKyEAQYASABEgL6kPD_BwE&amp;sig=AOD64_19iDcUmOV1dE0jzxI2s7kIk05fQA&amp;ctype=5&amp;q=&amp;ved=0ahUKEwiZktbc7b2AAxUYqpUCHUWoCdAQww8Ixww&amp;adurl=</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwiayt_c7b2AAxXIMdQBHZwOArIYABAFGgJvYQ&amp;gclid=EAIaIQobChMImsrf3O29gAMVyDHUAR2cDgKyEAQYAyABEgKk1vD_BwE&amp;sig=AOD64_0PCVkL9_zvI37E72iNAK74Co_etA&amp;ctype=5&amp;q=&amp;ved=0ahUKEwiZktbc7b2AAxUYqpUCHUWoCdAQww8Izww&amp;adurl=</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwiayt_c7b2AAxXIMdQBHZwOArIYABALGgJvYQ&amp;gclid=EAIaIQobChMImsrf3O29gAMVyDHUAR2cDgKyEAQYBiABEgI3kPD_BwE&amp;sig=AOD64_3v6AQScSRprx4HZxKVcGzIRmU_iA&amp;ctype=5&amp;q=&amp;ved=0ahUKEwiZktbc7b2AAxUYqpUCHUWoCdAQww8I2Qw&amp;adurl=</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwiayt_c7b2AAxXIMdQBHZwOArIYABAVGgJvYQ&amp;gclid=EAIaIQobChMImsrf3O29gAMVyDHUAR2cDgKyEAQYCyABEgJ8LPD_BwE&amp;sig=AOD64_1OGieLitwlQ2Pz4yOKeUTB5X98Ww&amp;ctype=5&amp;q=&amp;ved=0ahUKEwiZktbc7b2AAxUYqpUCHUWoCdAQww8I6ww&amp;adurl=</t>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABABGgJjZQ&amp;sig=AOD64_34DxrFXzasoPQwqJBjphAkiWOBSg&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQww8Iygw&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABAFGgJjZQ&amp;sig=AOD64_06IUnEVYQQMWu4wJ0xAqMo7FPmJA&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQww8I0gw&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABAVGgJjZQ&amp;sig=AOD64_3yM2MV16Dy7D6qYOiDspoYT7HoHg&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQww8I7gw&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABAnGgJjZQ&amp;sig=AOD64_3va6pzH4P3F3x7UHlfSnxAZYVP0A&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQ9A4I8hU&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABArGgJjZQ&amp;sig=AOD64_13bJwCwSmGwViYbGTl_1F3GPe9EA&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQ9A4I-RU&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABAtGgJjZQ&amp;sig=AOD64_2-LB9KA2AzKKtTUoPfzPIrPYQsAg&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQ9A4I_BU&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/aclk?sa=l&amp;ai=DChcSEwj9isjRy8GAAxVcQkgAHfvrDVUYABAvGgJjZQ&amp;sig=AOD64_3omzBLCWaDHRB9e48BnQ4AHFjw5w&amp;ctype=5&amp;q=&amp;ved=0ahUKEwjQj8PRy8GAAxUMp5UCHVsiAtYQ9A4I_xU&amp;adurl=</t>
   </si>
   <si>
     <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064%20gb</t>
@@ -429,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -454,7 +472,7 @@
         <v>3499</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -465,7 +483,7 @@
         <v>3349</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -476,7 +494,7 @@
         <v>3199</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -484,10 +502,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3499</v>
+        <v>3349</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -495,10 +513,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3171</v>
+        <v>3349</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -506,10 +524,43 @@
         <v>8</v>
       </c>
       <c r="B7">
+        <v>3199</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>3379</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>3023</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
         <v>4108.27</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -520,6 +571,9 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
     <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>